<commit_message>
Added repair option, events launcher, modified cards, and communicator to building phase
</commit_message>
<xml_diff>
--- a/modules/cardsnew.xlsx
+++ b/modules/cardsnew.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="240">
   <si>
     <t>card</t>
   </si>
@@ -294,9 +294,6 @@
     <t>damage_to_defenders</t>
   </si>
   <si>
-    <t>return_discarded</t>
-  </si>
-  <si>
     <t>discard_defender</t>
   </si>
   <si>
@@ -312,15 +309,9 @@
     <t>destroy_defender</t>
   </si>
   <si>
-    <t>destroy_defender + destroy_structure</t>
-  </si>
-  <si>
     <t>eliminate_damage</t>
   </si>
   <si>
-    <t>gain_money</t>
-  </si>
-  <si>
     <t>Supports Stargate</t>
   </si>
   <si>
@@ -721,6 +712,30 @@
   </si>
   <si>
     <t>Research_Labs</t>
+  </si>
+  <si>
+    <t>return_discarded_defender</t>
+  </si>
+  <si>
+    <t>return_discarded_building</t>
+  </si>
+  <si>
+    <t>gain_money_per_structure</t>
+  </si>
+  <si>
+    <t>gain_per_colony</t>
+  </si>
+  <si>
+    <t>gain_per_lab</t>
+  </si>
+  <si>
+    <t>halve_money</t>
+  </si>
+  <si>
+    <t>tax</t>
+  </si>
+  <si>
+    <t>gain_per_mine</t>
   </si>
 </sst>
 </file>
@@ -1061,11 +1076,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="L57" sqref="L57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="12" max="12" width="36.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
@@ -1084,22 +1102,22 @@
         <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G1" t="s">
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J1" t="s">
+        <v>105</v>
+      </c>
+      <c r="K1" t="s">
         <v>106</v>
-      </c>
-      <c r="I1" t="s">
-        <v>107</v>
-      </c>
-      <c r="J1" t="s">
-        <v>108</v>
-      </c>
-      <c r="K1" t="s">
-        <v>109</v>
       </c>
       <c r="L1" t="s">
         <v>7</v>
@@ -1108,19 +1126,19 @@
         <v>2</v>
       </c>
       <c r="N1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="O1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="P1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="Q1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="R1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="15.75">
@@ -1167,18 +1185,18 @@
         <v>5</v>
       </c>
       <c r="O2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="15.75">
       <c r="A3" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B3" t="s">
         <v>30</v>
@@ -1220,13 +1238,13 @@
         <v>1</v>
       </c>
       <c r="O3" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3" t="s">
         <v>110</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="15.75">
@@ -1273,13 +1291,13 @@
         <v>1</v>
       </c>
       <c r="O4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q4">
         <v>0</v>
       </c>
       <c r="R4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="15.75">
@@ -1326,13 +1344,13 @@
         <v>1</v>
       </c>
       <c r="O5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q5">
         <v>0</v>
       </c>
       <c r="R5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="15.75">
@@ -1379,13 +1397,13 @@
         <v>1</v>
       </c>
       <c r="O6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q6">
         <v>0</v>
       </c>
       <c r="R6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="15.75">
@@ -1432,13 +1450,13 @@
         <v>1</v>
       </c>
       <c r="O7" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q7">
         <v>0</v>
       </c>
       <c r="R7" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="15.75">
@@ -1485,13 +1503,13 @@
         <v>1</v>
       </c>
       <c r="O8" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q8">
         <v>0</v>
       </c>
       <c r="R8" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="15.75">
@@ -1538,18 +1556,18 @@
         <v>1</v>
       </c>
       <c r="O9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q9">
         <v>0</v>
       </c>
       <c r="R9" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="15.75">
       <c r="A10" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B10" t="s">
         <v>30</v>
@@ -1582,7 +1600,7 @@
         <v>1</v>
       </c>
       <c r="L10" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M10">
         <v>0</v>
@@ -1591,13 +1609,13 @@
         <v>1</v>
       </c>
       <c r="O10" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q10">
         <v>0</v>
       </c>
       <c r="R10" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="15.75">
@@ -1644,18 +1662,18 @@
         <v>1</v>
       </c>
       <c r="O11" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q11">
         <v>0</v>
       </c>
       <c r="R11" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="15.75">
       <c r="A12" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B12" t="s">
         <v>30</v>
@@ -1697,18 +1715,18 @@
         <v>1</v>
       </c>
       <c r="O12" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q12">
         <v>0</v>
       </c>
       <c r="R12" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="15.75">
       <c r="A13" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B13" t="s">
         <v>30</v>
@@ -1750,18 +1768,18 @@
         <v>1</v>
       </c>
       <c r="O13" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q13">
         <v>0</v>
       </c>
       <c r="R13" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="15.75">
       <c r="A14" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B14" t="s">
         <v>30</v>
@@ -1803,18 +1821,18 @@
         <v>3</v>
       </c>
       <c r="O14" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q14">
         <v>0</v>
       </c>
       <c r="R14" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="15.75">
       <c r="A15" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B15" t="s">
         <v>46</v>
@@ -1853,18 +1871,18 @@
         <v>2</v>
       </c>
       <c r="O15" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q15">
         <v>0</v>
       </c>
       <c r="R15" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="15.75">
       <c r="A16" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B16" t="s">
         <v>46</v>
@@ -1900,18 +1918,18 @@
         <v>2</v>
       </c>
       <c r="O16" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q16">
         <v>0</v>
       </c>
       <c r="R16" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="15.75">
       <c r="A17" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B17" t="s">
         <v>46</v>
@@ -1947,18 +1965,18 @@
         <v>3</v>
       </c>
       <c r="O17" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q17">
         <v>0</v>
       </c>
       <c r="R17" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:18" ht="15.75">
       <c r="A18" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B18" t="s">
         <v>46</v>
@@ -1994,18 +2012,18 @@
         <v>4</v>
       </c>
       <c r="O18" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q18">
         <v>0</v>
       </c>
       <c r="R18" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="15.75">
       <c r="A19" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B19" t="s">
         <v>46</v>
@@ -2041,18 +2059,18 @@
         <v>4</v>
       </c>
       <c r="O19" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q19">
         <v>0</v>
       </c>
       <c r="R19" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="15.75">
       <c r="A20" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B20" t="s">
         <v>46</v>
@@ -2088,18 +2106,18 @@
         <v>3</v>
       </c>
       <c r="O20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q20">
         <v>0</v>
       </c>
       <c r="R20" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:18" ht="15.75">
       <c r="A21" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B21" t="s">
         <v>46</v>
@@ -2135,18 +2153,18 @@
         <v>3</v>
       </c>
       <c r="O21" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q21">
         <v>0</v>
       </c>
       <c r="R21" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="1:18" ht="15.75">
       <c r="A22" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B22" t="s">
         <v>46</v>
@@ -2182,18 +2200,18 @@
         <v>1</v>
       </c>
       <c r="O22" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q22">
         <v>0</v>
       </c>
       <c r="R22" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="15.75">
       <c r="A23" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B23" t="s">
         <v>46</v>
@@ -2229,18 +2247,18 @@
         <v>3</v>
       </c>
       <c r="O23" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q23">
         <v>0</v>
       </c>
       <c r="R23" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="24" spans="1:18" ht="15.75">
       <c r="A24" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B24" t="s">
         <v>46</v>
@@ -2276,18 +2294,18 @@
         <v>2</v>
       </c>
       <c r="O24" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q24">
         <v>0</v>
       </c>
       <c r="R24" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="15.75">
       <c r="A25" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B25" t="s">
         <v>46</v>
@@ -2326,18 +2344,18 @@
         <v>2</v>
       </c>
       <c r="O25" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q25">
         <v>0</v>
       </c>
       <c r="R25" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="26" spans="1:18" ht="15.75">
       <c r="A26" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B26" t="s">
         <v>46</v>
@@ -2373,18 +2391,18 @@
         <v>3</v>
       </c>
       <c r="O26" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q26">
         <v>0</v>
       </c>
       <c r="R26" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="27" spans="1:18" ht="15.75">
       <c r="A27" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B27" t="s">
         <v>46</v>
@@ -2423,18 +2441,18 @@
         <v>5</v>
       </c>
       <c r="O27" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q27">
         <v>0</v>
       </c>
       <c r="R27" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="28" spans="1:18" ht="15.75">
       <c r="A28" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B28" t="s">
         <v>67</v>
@@ -2470,18 +2488,18 @@
         <v>3</v>
       </c>
       <c r="O28" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q28">
         <v>0</v>
       </c>
       <c r="R28" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:18" ht="15.75">
       <c r="A29" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B29" t="s">
         <v>67</v>
@@ -2517,18 +2535,18 @@
         <v>4</v>
       </c>
       <c r="O29" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q29">
         <v>0</v>
       </c>
       <c r="R29" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="15.75">
       <c r="A30" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B30" t="s">
         <v>67</v>
@@ -2564,18 +2582,18 @@
         <v>6</v>
       </c>
       <c r="O30" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q30">
         <v>0</v>
       </c>
       <c r="R30" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="15.75">
       <c r="A31" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B31" t="s">
         <v>67</v>
@@ -2611,18 +2629,18 @@
         <v>3</v>
       </c>
       <c r="O31" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q31">
         <v>0</v>
       </c>
       <c r="R31" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="32" spans="1:18" ht="15.75">
       <c r="A32" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B32" t="s">
         <v>67</v>
@@ -2658,18 +2676,18 @@
         <v>3</v>
       </c>
       <c r="O32" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q32">
         <v>0</v>
       </c>
       <c r="R32" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="33" spans="1:18" ht="15.75">
       <c r="A33" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B33" t="s">
         <v>67</v>
@@ -2705,18 +2723,18 @@
         <v>6</v>
       </c>
       <c r="O33" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q33">
         <v>0</v>
       </c>
       <c r="R33" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="34" spans="1:18" ht="15.75">
       <c r="A34" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B34" t="s">
         <v>67</v>
@@ -2752,18 +2770,18 @@
         <v>4</v>
       </c>
       <c r="O34" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q34">
         <v>0</v>
       </c>
       <c r="R34" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="35" spans="1:18" ht="15.75">
       <c r="A35" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B35" t="s">
         <v>67</v>
@@ -2799,18 +2817,18 @@
         <v>5</v>
       </c>
       <c r="O35" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q35">
         <v>0</v>
       </c>
       <c r="R35" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:18" ht="15.75">
       <c r="A36" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B36" t="s">
         <v>67</v>
@@ -2846,18 +2864,18 @@
         <v>3</v>
       </c>
       <c r="O36" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q36">
         <v>0</v>
       </c>
       <c r="R36" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="37" spans="1:18" ht="15.75">
       <c r="A37" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B37" t="s">
         <v>67</v>
@@ -2893,18 +2911,18 @@
         <v>4</v>
       </c>
       <c r="O37" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q37">
         <v>0</v>
       </c>
       <c r="R37" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="38" spans="1:18" ht="15.75">
       <c r="A38" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B38" t="s">
         <v>67</v>
@@ -2940,18 +2958,18 @@
         <v>3</v>
       </c>
       <c r="O38" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q38">
         <v>0</v>
       </c>
       <c r="R38" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="39" spans="1:18" ht="15.75">
       <c r="A39" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B39" t="s">
         <v>67</v>
@@ -2987,18 +3005,18 @@
         <v>6</v>
       </c>
       <c r="O39" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q39">
         <v>0</v>
       </c>
       <c r="R39" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="40" spans="1:18" ht="15.75">
       <c r="A40" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B40" t="s">
         <v>67</v>
@@ -3034,18 +3052,18 @@
         <v>4</v>
       </c>
       <c r="O40" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q40">
         <v>0</v>
       </c>
       <c r="R40" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="41" spans="1:18" ht="15.75">
       <c r="A41" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B41" t="s">
         <v>67</v>
@@ -3081,18 +3099,18 @@
         <v>5</v>
       </c>
       <c r="O41" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q41">
         <v>0</v>
       </c>
       <c r="R41" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="42" spans="1:18" ht="15.75">
       <c r="A42" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B42" t="s">
         <v>67</v>
@@ -3128,18 +3146,18 @@
         <v>5</v>
       </c>
       <c r="O42" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q42">
         <v>0</v>
       </c>
       <c r="R42" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="43" spans="1:18" ht="15.75">
       <c r="A43" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B43" t="s">
         <v>67</v>
@@ -3175,18 +3193,18 @@
         <v>4</v>
       </c>
       <c r="O43" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q43">
         <v>0</v>
       </c>
       <c r="R43" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="44" spans="1:18" ht="15.75">
       <c r="A44" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B44" t="s">
         <v>67</v>
@@ -3222,13 +3240,13 @@
         <v>3</v>
       </c>
       <c r="O44" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q44">
         <v>0</v>
       </c>
       <c r="R44" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="45" spans="1:18" ht="15.75">
@@ -3269,18 +3287,18 @@
         <v>6</v>
       </c>
       <c r="O45" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q45">
         <v>0</v>
       </c>
       <c r="R45" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="46" spans="1:18" ht="15.75">
       <c r="A46" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B46" t="s">
         <v>67</v>
@@ -3316,18 +3334,18 @@
         <v>3</v>
       </c>
       <c r="O46" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q46">
         <v>0</v>
       </c>
       <c r="R46" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="47" spans="1:18" ht="15.75">
       <c r="A47" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B47" t="s">
         <v>67</v>
@@ -3363,18 +3381,18 @@
         <v>7</v>
       </c>
       <c r="O47" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q47">
         <v>0</v>
       </c>
       <c r="R47" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="48" spans="1:18" ht="15.75">
       <c r="A48" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B48" t="s">
         <v>90</v>
@@ -3413,13 +3431,13 @@
         <v>0</v>
       </c>
       <c r="O48" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q48">
         <v>0</v>
       </c>
       <c r="R48" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="49" spans="1:18" ht="15.75">
@@ -3454,7 +3472,7 @@
         <v>0</v>
       </c>
       <c r="L49" t="s">
-        <v>92</v>
+        <v>232</v>
       </c>
       <c r="M49">
         <v>0</v>
@@ -3463,18 +3481,18 @@
         <v>0</v>
       </c>
       <c r="O49" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q49">
         <v>0</v>
       </c>
       <c r="R49" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="50" spans="1:18" ht="15.75">
       <c r="A50" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B50" t="s">
         <v>90</v>
@@ -3504,7 +3522,7 @@
         <v>0</v>
       </c>
       <c r="L50" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M50">
         <v>0</v>
@@ -3513,13 +3531,13 @@
         <v>0</v>
       </c>
       <c r="O50" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q50">
         <v>0</v>
       </c>
       <c r="R50" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="51" spans="1:18" ht="15.75">
@@ -3554,7 +3572,7 @@
         <v>0</v>
       </c>
       <c r="L51" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M51">
         <v>0</v>
@@ -3563,18 +3581,18 @@
         <v>0</v>
       </c>
       <c r="O51" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q51">
         <v>0</v>
       </c>
       <c r="R51" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="52" spans="1:18" ht="15.75">
       <c r="A52" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B52" t="s">
         <v>90</v>
@@ -3604,7 +3622,7 @@
         <v>0</v>
       </c>
       <c r="L52" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M52">
         <v>0</v>
@@ -3613,18 +3631,18 @@
         <v>0</v>
       </c>
       <c r="O52" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q52">
         <v>0</v>
       </c>
       <c r="R52" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="53" spans="1:18" ht="15.75">
       <c r="A53" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B53" t="s">
         <v>90</v>
@@ -3654,7 +3672,7 @@
         <v>0</v>
       </c>
       <c r="L53" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M53">
         <v>0</v>
@@ -3663,13 +3681,13 @@
         <v>0</v>
       </c>
       <c r="O53" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q53">
         <v>0</v>
       </c>
       <c r="R53" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="54" spans="1:18" ht="15.75">
@@ -3704,7 +3722,7 @@
         <v>0</v>
       </c>
       <c r="L54" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M54">
         <v>0</v>
@@ -3713,18 +3731,18 @@
         <v>0</v>
       </c>
       <c r="O54" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q54">
         <v>0</v>
       </c>
       <c r="R54" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="55" spans="1:18" ht="15.75">
       <c r="A55" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B55" t="s">
         <v>90</v>
@@ -3754,7 +3772,7 @@
         <v>0</v>
       </c>
       <c r="L55" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M55">
         <v>0</v>
@@ -3763,18 +3781,18 @@
         <v>0</v>
       </c>
       <c r="O55" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q55">
         <v>0</v>
       </c>
       <c r="R55" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="56" spans="1:18" ht="15.75">
       <c r="A56" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B56" t="s">
         <v>90</v>
@@ -3804,7 +3822,7 @@
         <v>0</v>
       </c>
       <c r="L56" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="M56">
         <v>0</v>
@@ -3813,18 +3831,18 @@
         <v>0</v>
       </c>
       <c r="O56" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q56">
         <v>0</v>
       </c>
       <c r="R56" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="57" spans="1:18" ht="15.75">
       <c r="A57" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B57" t="s">
         <v>90</v>
@@ -3854,7 +3872,7 @@
         <v>0</v>
       </c>
       <c r="L57" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="M57">
         <v>0</v>
@@ -3863,18 +3881,18 @@
         <v>0</v>
       </c>
       <c r="O57" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q57">
         <v>0</v>
       </c>
       <c r="R57" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="58" spans="1:18" ht="15.75">
       <c r="A58" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B58" t="s">
         <v>90</v>
@@ -3904,7 +3922,7 @@
         <v>0</v>
       </c>
       <c r="L58" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M58">
         <v>0</v>
@@ -3913,13 +3931,13 @@
         <v>0</v>
       </c>
       <c r="O58" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q58">
         <v>0</v>
       </c>
       <c r="R58" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="59" spans="1:18" ht="15.75">
@@ -3954,7 +3972,7 @@
         <v>0</v>
       </c>
       <c r="L59" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M59">
         <v>0</v>
@@ -3963,18 +3981,18 @@
         <v>0</v>
       </c>
       <c r="O59" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q59">
         <v>0</v>
       </c>
       <c r="R59" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="60" spans="1:18" ht="15.75">
       <c r="A60" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B60" t="s">
         <v>90</v>
@@ -4004,7 +4022,7 @@
         <v>0</v>
       </c>
       <c r="L60" t="s">
-        <v>100</v>
+        <v>239</v>
       </c>
       <c r="M60">
         <v>0</v>
@@ -4013,18 +4031,18 @@
         <v>0</v>
       </c>
       <c r="O60" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q60">
         <v>0</v>
       </c>
       <c r="R60" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="61" spans="1:18" ht="15.75">
       <c r="A61" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B61" t="s">
         <v>90</v>
@@ -4054,7 +4072,7 @@
         <v>0</v>
       </c>
       <c r="L61" t="s">
-        <v>100</v>
+        <v>234</v>
       </c>
       <c r="M61">
         <v>0</v>
@@ -4063,18 +4081,18 @@
         <v>0</v>
       </c>
       <c r="O61" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q61">
         <v>0</v>
       </c>
       <c r="R61" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="62" spans="1:18" ht="15.75">
       <c r="A62" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B62" t="s">
         <v>90</v>
@@ -4104,7 +4122,7 @@
         <v>0</v>
       </c>
       <c r="L62" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M62">
         <v>0</v>
@@ -4113,18 +4131,18 @@
         <v>0</v>
       </c>
       <c r="O62" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q62">
         <v>0</v>
       </c>
       <c r="R62" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="63" spans="1:18" ht="15.75">
       <c r="A63" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B63" t="s">
         <v>90</v>
@@ -4154,7 +4172,7 @@
         <v>0</v>
       </c>
       <c r="L63" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M63">
         <v>0</v>
@@ -4163,18 +4181,18 @@
         <v>0</v>
       </c>
       <c r="O63" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q63">
         <v>0</v>
       </c>
       <c r="R63" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="64" spans="1:18" ht="15.75">
       <c r="A64" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B64" t="s">
         <v>90</v>
@@ -4204,7 +4222,7 @@
         <v>0</v>
       </c>
       <c r="L64" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="M64">
         <v>0</v>
@@ -4213,13 +4231,13 @@
         <v>0</v>
       </c>
       <c r="O64" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q64">
         <v>0</v>
       </c>
       <c r="R64" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="65" spans="1:18" ht="15.75">
@@ -4254,7 +4272,7 @@
         <v>0</v>
       </c>
       <c r="L65" t="s">
-        <v>100</v>
+        <v>236</v>
       </c>
       <c r="M65">
         <v>0</v>
@@ -4263,18 +4281,18 @@
         <v>0</v>
       </c>
       <c r="O65" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q65">
         <v>0</v>
       </c>
       <c r="R65" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="66" spans="1:18" ht="15.75">
       <c r="A66" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B66" t="s">
         <v>90</v>
@@ -4304,7 +4322,7 @@
         <v>0</v>
       </c>
       <c r="L66" t="s">
-        <v>100</v>
+        <v>235</v>
       </c>
       <c r="M66">
         <v>0</v>
@@ -4313,18 +4331,18 @@
         <v>0</v>
       </c>
       <c r="O66" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q66">
         <v>0</v>
       </c>
       <c r="R66" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="67" spans="1:18" ht="15.75">
       <c r="A67" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B67" t="s">
         <v>90</v>
@@ -4354,7 +4372,7 @@
         <v>0</v>
       </c>
       <c r="L67" t="s">
-        <v>100</v>
+        <v>237</v>
       </c>
       <c r="M67">
         <v>0</v>
@@ -4363,18 +4381,18 @@
         <v>0</v>
       </c>
       <c r="O67" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q67">
         <v>0</v>
       </c>
       <c r="R67" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="68" spans="1:18" ht="15.75">
       <c r="A68" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B68" t="s">
         <v>90</v>
@@ -4404,7 +4422,7 @@
         <v>0</v>
       </c>
       <c r="L68" t="s">
-        <v>100</v>
+        <v>238</v>
       </c>
       <c r="M68">
         <v>0</v>
@@ -4413,13 +4431,13 @@
         <v>0</v>
       </c>
       <c r="O68" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q68">
         <v>0</v>
       </c>
       <c r="R68" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="69" spans="1:18" ht="15.75">
@@ -4454,7 +4472,7 @@
         <v>0</v>
       </c>
       <c r="L69" t="s">
-        <v>92</v>
+        <v>233</v>
       </c>
       <c r="M69">
         <v>0</v>
@@ -4463,13 +4481,13 @@
         <v>0</v>
       </c>
       <c r="O69" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q69">
         <v>0</v>
       </c>
       <c r="R69" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>